<commit_message>
Final & last changes #SNET-26
</commit_message>
<xml_diff>
--- a/users/Companies.xlsx
+++ b/users/Companies.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Propuesta" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="71">
   <si>
     <t>Nombre(s):</t>
   </si>
@@ -630,9 +631,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="58" width="9.19921875" style="2" customWidth="1"/>
+    <col min="59" max="16384" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3212401502</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3132084944</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3144781300</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -918,7 +1205,6 @@
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>